<commit_message>
Moving some functions to proper packages, other general cleanup stuff, starting to build out list filtering for the web page template.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -28,6 +28,9 @@
     <t>Is Outdated?</t>
   </si>
   <si>
+    <t>Group</t>
+  </si>
+  <si>
     <t>{{ Bower.Name }}</t>
   </si>
   <si>
@@ -42,6 +45,9 @@
   <si>
     <t>{{ Bower.Outdated }}</t>
   </si>
+  <si>
+    <t>{{ Bower.Group }}</t>
+  </si>
 </sst>
 </file>
 
@@ -50,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -66,13 +72,25 @@
       <color indexed="8"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b val="1"/>
+      <sz val="11"/>
+      <color indexed="9"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -91,16 +109,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </left>
       <right style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="11"/>
       </bottom>
       <diagonal/>
     </border>
@@ -110,17 +128,23 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -141,6 +165,7 @@
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffa7a7a7"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -1209,9 +1234,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="2" width="8.85156" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.8516" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.8516" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="1" customWidth="1"/>
+    <col min="3" max="3" width="20" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.8516" style="1" customWidth="1"/>
     <col min="5" max="12" width="8.85156" style="1" customWidth="1"/>
     <col min="13" max="256" width="8.85156" style="1" customWidth="1"/>
   </cols>
@@ -1233,218 +1259,222 @@
         <v>4</v>
       </c>
       <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
+      <c r="G1" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
     <row r="2" ht="15" customHeight="1">
-      <c r="A2" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="B2" t="s" s="2">
+      <c r="A2" t="s" s="5">
         <v>6</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="B2" t="s" s="5">
         <v>7</v>
       </c>
-      <c r="D2" t="s" s="2">
+      <c r="C2" t="s" s="5">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="2">
+      <c r="D2" t="s" s="5">
         <v>9</v>
       </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="E2" t="s" s="5">
+        <v>10</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" t="s" s="5">
+        <v>11</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="3" ht="15" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
     <row r="4" ht="15" customHeight="1">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
     <row r="6" ht="15" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="4"/>
+      <c r="L6" s="4"/>
     </row>
     <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
     </row>
     <row r="8" ht="15" customHeight="1">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" ht="15" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4"/>
+      <c r="L9" s="4"/>
     </row>
     <row r="10" ht="15" customHeight="1">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" ht="15" customHeight="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" ht="15" customHeight="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="4"/>
     </row>
     <row r="14" ht="15" customHeight="1">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" ht="15" customHeight="1">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>